<commit_message>
bug 59814: clear evaluation workbook and evaluation sheet caches. Patch from Greg Woolsey.
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1751836 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/StructuredReferences.xlsx
+++ b/test-data/spreadsheet/StructuredReferences.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Formulas" sheetId="2" r:id="rId1"/>
     <sheet name="Table" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -203,6 +203,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -238,6 +255,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -390,9 +424,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -402,6 +438,18 @@
         <v>209</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>\_Prime.1[Name]</f>
+        <v>one</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>\_Prime.1[Name]</f>
+        <v>two</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -412,7 +460,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>